<commit_message>
Worked on releases #The following packages are "defined" # 1) RR_FULL    - This is a full release, containing everything # 2) RR_CXX     - C++ Distribution, contains relevant CXX files and libs and apps # 3) RR_C_API   - C API Distribution, contains relevant C API files # 4) RR_PYTHON  - Python API Distribution # 5) RR_DELPHI  - Delphi Distribution
nleq should be tested

Added a StopWatch

added bat files that cleans, makes and installs the CodeGear releases

Removed some obsolete files
</commit_message>
<xml_diff>
--- a/Misc/TestSuiteReports/failedTests_xel.xlsx
+++ b/Misc/TestSuiteReports/failedTests_xel.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\roadrunnerwork\Misc\TestSuiteReports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25830" windowHeight="13005"/>
   </bookViews>
   <sheets>
     <sheet name="failedTests_xe_Excel" sheetId="1" r:id="rId1"/>
@@ -148,8 +153,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -983,21 +988,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A2:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
@@ -1014,7 +1022,7 @@
     <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M2" s="1" t="s">
         <v>30</v>
       </c>
@@ -1025,7 +1033,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="3" customFormat="1" ht="45">
+    <row r="3" spans="1:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1063,7 +1071,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="3" customFormat="1">
+    <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1099,7 +1107,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="3" customFormat="1">
+    <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1135,7 +1143,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="3" customFormat="1">
+    <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1168,7 +1176,7 @@
       </c>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:19" s="3" customFormat="1">
+    <row r="7" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1209,7 +1217,7 @@
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
     </row>
-    <row r="8" spans="1:19" s="10" customFormat="1">
+    <row r="8" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
@@ -1244,7 +1252,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="30">
+    <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1279,7 +1287,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1314,7 +1322,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="14" customFormat="1">
+    <row r="11" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
@@ -1351,7 +1359,7 @@
       <c r="N11" s="12"/>
       <c r="O11" s="13"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
@@ -1390,7 +1398,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
@@ -1429,7 +1437,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="30">
+    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
@@ -1468,7 +1476,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>34</v>
       </c>
@@ -1484,7 +1492,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>38</v>
       </c>
@@ -1498,7 +1506,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
@@ -1530,7 +1538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>35</v>
       </c>
@@ -1546,7 +1554,7 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>36</v>
       </c>
@@ -1560,7 +1568,7 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -1592,7 +1600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
@@ -1624,7 +1632,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -1656,7 +1664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
@@ -1688,7 +1696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -1720,7 +1728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1757,6 +1765,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="47" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enabled eventPriorities array Added a new class rrEvent, that correspond to a simple event representation. It can be sorted in an Array Worked on SortEvenPriorities
Enabled some randomness..
Cleaned up some c code generation

This revision made model 892, 931 934 936 to pass
new models NOT passing are 935 952 964 965 966
</commit_message>
<xml_diff>
--- a/Misc/TestSuiteReports/failedTests_xel.xlsx
+++ b/Misc/TestSuiteReports/failedTests_xel.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="39">
   <si>
     <t>FAIL</t>
   </si>
@@ -66,15 +66,6 @@
     <t>KNOWN_PROBLEM</t>
   </si>
   <si>
-    <t>Case_892</t>
-  </si>
-  <si>
-    <t>Case_931</t>
-  </si>
-  <si>
-    <t>Case_934</t>
-  </si>
-  <si>
     <t>Case_936</t>
   </si>
   <si>
@@ -141,13 +132,10 @@
     <t>S3 wrong init conc</t>
   </si>
   <si>
-    <t>Initial conc. seem ok. S2 donet evolve as model</t>
-  </si>
-  <si>
-    <t>Todo. Sort event priorities</t>
-  </si>
-  <si>
     <t>sinus and spf_piecewise need #args</t>
+  </si>
+  <si>
+    <t>Initial conc. seem ok. S2 dont evolve as model</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +990,7 @@
   <dimension ref="A2:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,13 +1012,13 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1065,10 +1053,10 @@
         <v>5</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1104,7 +1092,7 @@
       </c>
       <c r="O4" s="4"/>
       <c r="S4" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1140,7 +1128,7 @@
       </c>
       <c r="O5" s="4"/>
       <c r="S5" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1249,7 +1237,7 @@
         <v>5</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
@@ -1284,7 +1272,7 @@
         <v>5</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1319,40 +1307,20 @@
         <v>5</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="12">
-        <v>87</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="12">
-        <v>6.4080500000000002E-3</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>5</v>
-      </c>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
@@ -1360,86 +1328,42 @@
       <c r="O11" s="13"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="6">
-        <v>78</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="6">
-        <v>3</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
-      <c r="O12" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="O12" s="8"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6">
-        <v>52</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="6">
-        <v>1</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="O13" s="8"/>
     </row>
     <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>0</v>
@@ -1473,12 +1397,12 @@
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>0</v>
@@ -1494,7 +1418,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1508,7 +1432,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>0</v>
@@ -1540,7 +1464,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>0</v>
@@ -1556,7 +1480,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1570,7 +1494,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>0</v>
@@ -1602,7 +1526,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>0</v>
@@ -1634,7 +1558,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>0</v>
@@ -1666,7 +1590,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>0</v>
@@ -1698,7 +1622,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>0</v>
@@ -1730,7 +1654,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>0</v>
@@ -1760,7 +1684,7 @@
         <v>5</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a problem in XE ? operator  strikes = (tooCloseToStart) ? 3 : strikes--; Don't work!
Caused some models to get into an endless loop ..

Updated KnownProblems wiki with all failing models
</commit_message>
<xml_diff>
--- a/Misc/TestSuiteReports/failedTests_xel.xlsx
+++ b/Misc/TestSuiteReports/failedTests_xel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25830" windowHeight="13005"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9960"/>
   </bookViews>
   <sheets>
     <sheet name="failedTests_xe_Excel" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="39">
   <si>
     <t>FAIL</t>
   </si>
@@ -66,9 +66,6 @@
     <t>KNOWN_PROBLEM</t>
   </si>
   <si>
-    <t>Case_936</t>
-  </si>
-  <si>
     <t>Case_955</t>
   </si>
   <si>
@@ -132,10 +129,13 @@
     <t>S3 wrong init conc</t>
   </si>
   <si>
-    <t>sinus and spf_piecewise need #args</t>
-  </si>
-  <si>
     <t>Initial conc. seem ok. S2 dont evolve as model</t>
+  </si>
+  <si>
+    <t>Case 748</t>
+  </si>
+  <si>
+    <t>infinity stuff</t>
   </si>
 </sst>
 </file>
@@ -987,10 +987,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:S25"/>
+  <dimension ref="A2:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,13 +1012,13 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="S2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1053,10 +1053,10 @@
         <v>5</v>
       </c>
       <c r="O3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1092,7 +1092,7 @@
       </c>
       <c r="O4" s="4"/>
       <c r="S4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1128,7 +1128,7 @@
       </c>
       <c r="O5" s="4"/>
       <c r="S5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1237,7 +1237,7 @@
         <v>5</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
@@ -1272,7 +1272,7 @@
         <v>5</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1307,7 +1307,7 @@
         <v>5</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,9 @@
       <c r="O11" s="13"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="6">
+        <v>374</v>
+      </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -1345,7 +1347,9 @@
       <c r="O12" s="8"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -1361,52 +1365,28 @@
       <c r="N13" s="6"/>
       <c r="O13" s="8"/>
     </row>
-    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="6">
-        <v>194</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="6">
-        <v>3</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H14" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="8" t="s">
-        <v>37</v>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="M14" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>0</v>
-      </c>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1418,7 +1398,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1431,58 +1411,58 @@
       <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="6">
-        <v>1</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="A17" s="6">
+        <v>952</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1494,39 +1474,21 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="6">
-        <v>171</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="6">
-        <v>1000</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>5</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>0</v>
@@ -1535,13 +1497,13 @@
         <v>1</v>
       </c>
       <c r="D21" s="6">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F21" s="6">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>3</v>
@@ -1553,12 +1515,12 @@
         <v>4</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>0</v>
@@ -1567,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="6">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>2</v>
@@ -1585,12 +1547,12 @@
         <v>4</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>0</v>
@@ -1599,13 +1561,13 @@
         <v>1</v>
       </c>
       <c r="D23" s="6">
-        <v>1999</v>
+        <v>11</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F23" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>3</v>
@@ -1622,7 +1584,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>0</v>
@@ -1631,13 +1593,13 @@
         <v>1</v>
       </c>
       <c r="D24" s="6">
-        <v>202</v>
+        <v>1999</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F24" s="6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>3</v>
@@ -1653,38 +1615,112 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="A25" s="6">
+        <v>964</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>965</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>966</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6">
+        <v>202</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="1">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="F28" s="6">
+        <v>5</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1" t="s">
+      <c r="H28" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>34</v>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>